<commit_message>
Added probability rows for true angle 1, 2, 8, and 9
</commit_message>
<xml_diff>
--- a/Assignment_6/Probability_table.xlsx
+++ b/Assignment_6/Probability_table.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{52C024ED-2EE1-4339-AE83-0B8C4F1D945C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{58D034F7-1F38-4E0D-9B8B-070B3FD5122B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +127,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -140,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -170,6 +176,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,9 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -617,14 +622,14 @@
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
+      <c r="C11" s="13">
+        <v>0.7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.1</v>
       </c>
       <c r="F11" s="4">
         <v>0</v>
@@ -650,17 +655,17 @@
       <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="4">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
-        <v>0</v>
+      <c r="C12" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.1</v>
       </c>
       <c r="G12" s="4">
         <v>0</v>
@@ -863,17 +868,17 @@
       <c r="G18" s="4">
         <v>0</v>
       </c>
-      <c r="H18" s="4">
-        <v>0</v>
-      </c>
-      <c r="I18" s="4">
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
-        <v>0</v>
-      </c>
-      <c r="K18" s="4">
-        <v>0</v>
+      <c r="H18" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="K18" s="13">
+        <v>0.3</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -901,14 +906,14 @@
       <c r="H19" s="4">
         <v>0</v>
       </c>
-      <c r="I19" s="4">
-        <v>0</v>
-      </c>
-      <c r="J19" s="4">
-        <v>0</v>
-      </c>
-      <c r="K19" s="4">
-        <v>0</v>
+      <c r="I19" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="K19" s="13">
+        <v>0.7</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>

</xml_diff>

<commit_message>
Added some more probability values in sheet2
</commit_message>
<xml_diff>
--- a/Assignment_6/Probability_table.xlsx
+++ b/Assignment_6/Probability_table.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{58D034F7-1F38-4E0D-9B8B-070B3FD5122B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DC996B6C-7371-4156-A24C-AFBBF7C0CD3E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="28">
   <si>
     <t>a</t>
   </si>
@@ -85,6 +86,45 @@
   </si>
   <si>
     <t>p(measured_angle | angle)</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>RIAA</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>RILA</t>
+  </si>
+  <si>
+    <t>1/9</t>
+  </si>
+  <si>
+    <t>4/9</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3/9</t>
+  </si>
+  <si>
+    <t>6/9</t>
+  </si>
+  <si>
+    <t>8/9</t>
+  </si>
+  <si>
+    <t>5/9</t>
+  </si>
+  <si>
+    <t>Outer Angles</t>
+  </si>
+  <si>
+    <t>Errors</t>
   </si>
 </sst>
 </file>
@@ -146,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -164,6 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -176,7 +217,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,20 +545,20 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -540,7 +590,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
@@ -574,17 +624,17 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C10" s="2">
@@ -616,13 +666,13 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="9">
         <v>0.7</v>
       </c>
       <c r="D11" s="3">
@@ -651,11 +701,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+      <c r="A12" s="11"/>
       <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="9">
         <v>0.3</v>
       </c>
       <c r="D12" s="3">
@@ -684,7 +734,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="11"/>
       <c r="B13" s="5">
         <v>3</v>
       </c>
@@ -717,7 +767,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
+      <c r="A14" s="11"/>
       <c r="B14" s="5">
         <v>4</v>
       </c>
@@ -750,7 +800,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
+      <c r="A15" s="11"/>
       <c r="B15" s="5">
         <v>5</v>
       </c>
@@ -783,7 +833,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
+      <c r="A16" s="11"/>
       <c r="B16" s="5">
         <v>6</v>
       </c>
@@ -816,7 +866,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
+      <c r="A17" s="11"/>
       <c r="B17" s="5">
         <v>7</v>
       </c>
@@ -849,7 +899,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="10"/>
+      <c r="A18" s="11"/>
       <c r="B18" s="1">
         <v>8</v>
       </c>
@@ -877,14 +927,14 @@
       <c r="J18" s="3">
         <v>0.39999999999999991</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="9">
         <v>0.3</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
+      <c r="A19" s="11"/>
       <c r="B19" s="1">
         <v>9</v>
       </c>
@@ -912,7 +962,7 @@
       <c r="J19" s="3">
         <v>0.2</v>
       </c>
-      <c r="K19" s="13">
+      <c r="K19" s="9">
         <v>0.7</v>
       </c>
       <c r="N19" s="4"/>
@@ -928,4 +978,428 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABDAD71-2F90-48E5-AA81-FA1527C77326}">
+  <dimension ref="A2:H27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3">
+        <v>50</v>
+      </c>
+      <c r="H3">
+        <f>SUM(C3:G3)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>30</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H6" si="0">SUM(C4:G4)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>30</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="14">
+        <v>0</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0</v>
+      </c>
+      <c r="E10" s="14">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14">
+        <v>3</v>
+      </c>
+      <c r="G10" s="14">
+        <v>5</v>
+      </c>
+      <c r="H10" s="14">
+        <f>SUM(C10:G10)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14">
+        <v>3</v>
+      </c>
+      <c r="F11" s="14">
+        <v>2</v>
+      </c>
+      <c r="G11" s="14">
+        <v>1</v>
+      </c>
+      <c r="H11" s="14">
+        <f t="shared" ref="H11:H13" si="1">SUM(C11:G11)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14">
+        <v>2</v>
+      </c>
+      <c r="E12" s="14">
+        <v>3</v>
+      </c>
+      <c r="F12" s="14">
+        <v>2</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1</v>
+      </c>
+      <c r="H12" s="14">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="14">
+        <v>5</v>
+      </c>
+      <c r="D13" s="14">
+        <v>3</v>
+      </c>
+      <c r="E13" s="14">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14">
+        <v>0</v>
+      </c>
+      <c r="G13" s="14">
+        <v>0</v>
+      </c>
+      <c r="H13" s="14">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C17" s="15">
+        <v>3</v>
+      </c>
+      <c r="D17" s="15">
+        <v>4</v>
+      </c>
+      <c r="E17" s="15">
+        <v>5</v>
+      </c>
+      <c r="F17" s="15">
+        <v>6</v>
+      </c>
+      <c r="G17" s="15">
+        <v>7</v>
+      </c>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="16">
+        <v>0</v>
+      </c>
+      <c r="D18" s="16">
+        <v>0</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="16">
+        <v>1</v>
+      </c>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="16">
+        <v>1</v>
+      </c>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="16">
+        <v>1</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0</v>
+      </c>
+      <c r="G21" s="16">
+        <v>0</v>
+      </c>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24" s="17">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <f>SUM(C24:G24)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>0.1</v>
+      </c>
+      <c r="D27">
+        <v>0.3</v>
+      </c>
+      <c r="E27">
+        <v>0.7</v>
+      </c>
+      <c r="F27">
+        <v>0.9</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>